<commit_message>
20191029 ejercicios si y - o
</commit_message>
<xml_diff>
--- a/m1/u1/ejercicios/20191028/Funciones lógicas/Ejercicios Y - O.xlsx
+++ b/m1/u1/ejercicios/20191028/Funciones lógicas/Ejercicios Y - O.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\Funciones lógicas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndresRamos\Documents\poo\m1\u1\ejercicios\20191028\Funciones lógicas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15045" windowHeight="5775" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Caso 2" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="111">
   <si>
     <t>Pertenecer al turno mañana.</t>
   </si>
@@ -378,6 +378,9 @@
   <si>
     <t>En la columna situación aparecerá "Cambiar Sección" en los empleados que cumplan ambas condiciones 
 y "Mantener puesto" en los que no</t>
+  </si>
+  <si>
+    <t>NO COBRA</t>
   </si>
 </sst>
 </file>
@@ -542,7 +545,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -604,11 +607,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -917,13 +921,13 @@
   <dimension ref="A3:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -956,7 +960,7 @@
       <c r="A7" s="7"/>
     </row>
     <row r="8" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="33" t="s">
         <v>109</v>
       </c>
     </row>
@@ -999,7 +1003,10 @@
       <c r="F12" s="2">
         <v>1</v>
       </c>
-      <c r="G12" s="11"/>
+      <c r="G12" s="11" t="str">
+        <f>IF(OR(AND(D12="M",F12=4),E12&lt;=7000),"CAMBIAR SECCION","MANTENER PUESTO")</f>
+        <v>MANTENER PUESTO</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
@@ -1017,7 +1024,10 @@
       <c r="F13" s="2">
         <v>4</v>
       </c>
-      <c r="G13" s="11"/>
+      <c r="G13" s="11" t="str">
+        <f t="shared" ref="G13:G22" si="0">IF(OR(AND(D13="M",F13=4),E13&lt;=7000),"CAMBIAR SECCION","MANTENER PUESTO")</f>
+        <v>CAMBIAR SECCION</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
@@ -1035,7 +1045,10 @@
       <c r="F14" s="2">
         <v>2</v>
       </c>
-      <c r="G14" s="11"/>
+      <c r="G14" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>CAMBIAR SECCION</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
@@ -1053,7 +1066,10 @@
       <c r="F15" s="2">
         <v>1</v>
       </c>
-      <c r="G15" s="11"/>
+      <c r="G15" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>CAMBIAR SECCION</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
@@ -1071,7 +1087,10 @@
       <c r="F16" s="2">
         <v>1</v>
       </c>
-      <c r="G16" s="11"/>
+      <c r="G16" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>MANTENER PUESTO</v>
+      </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
@@ -1089,7 +1108,10 @@
       <c r="F17" s="2">
         <v>3</v>
       </c>
-      <c r="G17" s="11"/>
+      <c r="G17" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>MANTENER PUESTO</v>
+      </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
@@ -1107,7 +1129,10 @@
       <c r="F18" s="2">
         <v>4</v>
       </c>
-      <c r="G18" s="11"/>
+      <c r="G18" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>CAMBIAR SECCION</v>
+      </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
@@ -1125,7 +1150,10 @@
       <c r="F19" s="2">
         <v>1</v>
       </c>
-      <c r="G19" s="11"/>
+      <c r="G19" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>CAMBIAR SECCION</v>
+      </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
@@ -1143,7 +1171,10 @@
       <c r="F20" s="2">
         <v>2</v>
       </c>
-      <c r="G20" s="11"/>
+      <c r="G20" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>MANTENER PUESTO</v>
+      </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
@@ -1161,7 +1192,10 @@
       <c r="F21" s="2">
         <v>2</v>
       </c>
-      <c r="G21" s="11"/>
+      <c r="G21" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>MANTENER PUESTO</v>
+      </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
@@ -1179,7 +1213,10 @@
       <c r="F22" s="2">
         <v>1</v>
       </c>
-      <c r="G22" s="11"/>
+      <c r="G22" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>MANTENER PUESTO</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -1193,12 +1230,13 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -1249,7 +1287,10 @@
         <f>D4/(E4*E4)</f>
         <v>21.907582457706194</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="13" t="str">
+        <f>IF(F4&lt;18,$A$13,IF(F4&lt;25,$A$14,IF(F4&lt;30,$A$15,IF(F4&lt;35,$A$16,IF(F4&lt;=40,$A$17,IF(F4&gt;40,$A$18))))))</f>
+        <v>normal</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
@@ -1271,7 +1312,10 @@
         <f>D5/(E5*E5)</f>
         <v>25.351541373715524</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="13" t="str">
+        <f t="shared" ref="G5:G10" si="0">IF(F5&lt;18,$A$13,IF(F5&lt;25,$A$14,IF(F5&lt;30,$A$15,IF(F5&lt;35,$A$16,IF(F5&lt;=40,$A$17,IF(F5&gt;40,$A$18))))))</f>
+        <v>sobre peso</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
@@ -1293,7 +1337,10 @@
         <f>D6/(E6*E6)</f>
         <v>30.863006828440259</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>morbido I</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
@@ -1315,7 +1362,10 @@
         <f>D7/(E7*E7)</f>
         <v>29.402273297715947</v>
       </c>
-      <c r="G7" s="2"/>
+      <c r="G7" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>sobre peso</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
@@ -1337,7 +1387,10 @@
         <f>D8/(E8*E8)</f>
         <v>36.982248520710058</v>
       </c>
-      <c r="G8" s="2"/>
+      <c r="G8" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>Morbido II</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
@@ -1358,7 +1411,10 @@
       <c r="F9" s="14">
         <v>17</v>
       </c>
-      <c r="G9" s="2"/>
+      <c r="G9" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>bajo peso</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
@@ -1379,7 +1435,10 @@
       <c r="F10" s="14">
         <v>40</v>
       </c>
-      <c r="G10" s="2"/>
+      <c r="G10" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>Morbido II</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
@@ -1452,13 +1511,14 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1511,7 +1571,10 @@
         <v>73</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="D10" s="36">
+        <f>IF(A10="OTRO","SIN DESCUENTO",IF(AND(A10="MAYORISTA",B10="CONTADO"),20%,IF(AND(A10="MINORISTA",B10="CONTADO"),10%,IF(AND(A10="MAYORISTA",B10="CREDITO"),15%,"SIN DESCUENTO"))))</f>
+        <v>0.2</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -1521,7 +1584,10 @@
         <v>71</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="D11" s="36">
+        <f t="shared" ref="D11:D14" si="0">IF(A11="OTRO","SIN DESCUENTO",IF(AND(A11="MAYORISTA",B11="CONTADO"),20%,IF(AND(A11="MINORISTA",B11="CONTADO"),10%,IF(AND(A11="MAYORISTA",B11="CREDITO"),15%,"SIN DESCUENTO"))))</f>
+        <v>0.15</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1531,7 +1597,10 @@
         <v>73</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="D12" s="36">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -1541,7 +1610,10 @@
         <v>71</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="D13" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>SIN DESCUENTO</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -1551,7 +1623,10 @@
         <v>73</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="D14" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>SIN DESCUENTO</v>
+      </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
@@ -1571,14 +1646,16 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="9" width="12.7109375" customWidth="1"/>
+    <col min="3" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
@@ -1658,7 +1735,10 @@
         <f t="shared" ref="G9:G14" si="0">AVERAGE(D9:F9)</f>
         <v>14</v>
       </c>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2" t="str">
+        <f>IF(AND(C9&gt;=80,G9&gt;=10.5),"APROBADO",IF(AND(C9&gt;=80,G9&lt;10.5),"RECUPERACION","DESAPROBADO"))</f>
+        <v>APROBADO</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
@@ -1680,7 +1760,10 @@
         <f t="shared" si="0"/>
         <v>9.3333333333333339</v>
       </c>
-      <c r="H10" s="2"/>
+      <c r="H10" s="2" t="str">
+        <f t="shared" ref="H10:H14" si="1">IF(AND(C10&gt;=80,G10&gt;=10.5),"APROBADO",IF(AND(C10&gt;=80,G10&lt;10.5),"RECUPERACION","DESAPROBADO"))</f>
+        <v>RECUPERACION</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
@@ -1702,7 +1785,10 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H11" s="2"/>
+      <c r="H11" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>DESAPROBADO</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
@@ -1724,7 +1810,10 @@
         <f t="shared" si="0"/>
         <v>9.6666666666666661</v>
       </c>
-      <c r="H12" s="2"/>
+      <c r="H12" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>RECUPERACION</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
@@ -1746,7 +1835,10 @@
         <f t="shared" si="0"/>
         <v>15.666666666666666</v>
       </c>
-      <c r="H13" s="2"/>
+      <c r="H13" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>APROBADO</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="27" t="s">
@@ -1768,7 +1860,10 @@
         <f t="shared" si="0"/>
         <v>10.333333333333334</v>
       </c>
-      <c r="H14" s="2"/>
+      <c r="H14" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>DESAPROBADO</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -1782,13 +1877,14 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
@@ -1806,53 +1902,53 @@
       <c r="A5" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="30" t="s">
@@ -1872,7 +1968,16 @@
       <c r="C11" s="2">
         <v>100</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2" t="str">
+        <f>IF(AND(C11&gt;99.5,C11&lt;=100),"COBRA 1000 EUROS",IF(AND(C11&gt;=99,C11&lt;99.5),"COBRA 900 EUROS",IF(AND(C11&gt;=98.5,C11&lt;99),"COBRA 800 EUROS","NO COBRA NADA")))</f>
+        <v>COBRA 1000 EUROS</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1000</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
@@ -1881,7 +1986,16 @@
       <c r="C12" s="2">
         <v>99.1</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2" t="str">
+        <f t="shared" ref="D12:D16" si="0">IF(AND(C12&gt;99.5,C12&lt;=100),"COBRA 1000 EUROS",IF(AND(C12&gt;=99,C12&lt;99.5),"COBRA 900 EUROS",IF(AND(C12&gt;=98.5,C12&lt;99),"COBRA 800 EUROS","NO COBRA NADA")))</f>
+        <v>COBRA 900 EUROS</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>900</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
@@ -1890,7 +2004,16 @@
       <c r="C13" s="2">
         <v>97</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>NO COBRA NADA</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
@@ -1899,7 +2022,16 @@
       <c r="C14" s="2">
         <v>98</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>NO COBRA NADA</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
@@ -1908,7 +2040,16 @@
       <c r="C15" s="2">
         <v>99.7</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>COBRA 1000 EUROS</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1000</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="27" t="s">
@@ -1917,7 +2058,16 @@
       <c r="C16" s="2">
         <v>98.8</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>COBRA 800 EUROS</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16">
+        <v>800</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>